<commit_message>
just logging my hcluster code
</commit_message>
<xml_diff>
--- a/Hcluster/files_for_dup.xlsx
+++ b/Hcluster/files_for_dup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24923"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,10 +15,19 @@
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -184,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,259 +510,259 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:1">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:1">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:1">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:1">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:1">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="30" spans="1:1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="31" spans="1:1">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.65">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>50</v>
       </c>

</xml_diff>